<commit_message>
Worked on age date
Worked on some more of the age data of the specimens
</commit_message>
<xml_diff>
--- a/BEAST2/Data/Pterosaur ages_11-23.xlsx
+++ b/BEAST2/Data/Pterosaur ages_11-23.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joël\Documents\GitHub\PterosaurPhylogeny\BEAST2\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\revbayes-v1.2.1-win64\revbayes-v1.2.1\Files\PterosaurPhylogeny\BEAST2\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B27FECA4-DA54-45C2-ACFC-D2425F815DD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35B13142-F474-4F31-A60D-351A1947AC29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15360" yWindow="0" windowWidth="15360" windowHeight="16680" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Defined ages" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="258">
   <si>
     <t>Age</t>
   </si>
@@ -810,6 +810,12 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>Carniadactylus rosenfeldi -2</t>
+  </si>
+  <si>
+    <t>Carniadactylus rosenfeldi -1</t>
   </si>
 </sst>
 </file>
@@ -849,7 +855,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="22">
+  <fills count="23">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -976,6 +982,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -1004,7 +1016,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1040,6 +1052,7 @@
     <xf numFmtId="0" fontId="4" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -1327,8 +1340,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H42" sqref="H42"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1789,8 +1802,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73C28F51-8982-4167-BE7A-7475AE363CAF}">
   <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1846,10 +1859,10 @@
       <c r="B2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="31" t="s">
         <v>58</v>
       </c>
       <c r="E2" s="12">
@@ -1881,10 +1894,10 @@
       <c r="B3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="25" t="s">
+      <c r="C3" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="D3" s="31" t="s">
         <v>72</v>
       </c>
       <c r="E3" s="15">
@@ -1916,10 +1929,10 @@
       <c r="B4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="25" t="s">
+      <c r="C4" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="31" t="s">
         <v>72</v>
       </c>
       <c r="E4" s="15">
@@ -1951,17 +1964,17 @@
       <c r="B5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="D5" t="s">
-        <v>85</v>
+      <c r="D5" s="31" t="s">
+        <v>81</v>
       </c>
       <c r="E5" s="15">
         <v>159.27000000000001</v>
       </c>
-      <c r="F5" s="14">
-        <v>154.78</v>
+      <c r="F5" s="15">
+        <v>157.01</v>
       </c>
       <c r="G5" t="s">
         <v>80</v>
@@ -1986,10 +1999,10 @@
       <c r="B6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="31" t="s">
         <v>5</v>
       </c>
       <c r="E6" s="14">
@@ -2016,19 +2029,19 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>37</v>
+        <v>257</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C7" t="s">
-        <v>72</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="C7" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="E7" s="15">
-        <v>217.49</v>
+      <c r="D7" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="E7" s="14">
+        <v>214.03</v>
       </c>
       <c r="F7" s="14">
         <v>209.51</v>
@@ -2566,10 +2579,10 @@
       <c r="B24" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="31" t="s">
         <v>84</v>
       </c>
       <c r="E24" s="15">
@@ -2671,10 +2684,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8BF1638-D451-49C3-A187-7D7621821287}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2688,7 +2701,7 @@
     <col min="9" max="9" width="36.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>164</v>
       </c>
@@ -2717,17 +2730,17 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>165</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="31" t="s">
         <v>84</v>
       </c>
       <c r="E2" s="14">
@@ -2746,178 +2759,213 @@
         <v>183</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E3" s="14">
+        <v>214.03</v>
+      </c>
+      <c r="F3" s="14">
+        <v>209.51</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="H3" t="s">
+        <v>93</v>
+      </c>
+      <c r="I3" s="16" t="s">
+        <v>185</v>
+      </c>
+      <c r="K3" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="L3" s="17" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>4</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D4" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="20">
+      <c r="E4" s="20">
         <v>227.3</v>
       </c>
-      <c r="F3" s="20">
+      <c r="F4" s="20">
         <v>209.51</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G4" t="s">
         <v>214</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H4" t="s">
         <v>213</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I4" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
         <v>168</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4" t="s">
-        <v>72</v>
-      </c>
-      <c r="D4" t="s">
-        <v>84</v>
-      </c>
-      <c r="E4" s="15">
-        <v>217.49</v>
-      </c>
-      <c r="F4" s="14">
-        <v>209.51</v>
-      </c>
-      <c r="G4" t="s">
-        <v>212</v>
-      </c>
-      <c r="H4" t="s">
-        <v>215</v>
-      </c>
-      <c r="I4" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
-        <v>169</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E5" s="15">
+        <v>217.49</v>
+      </c>
+      <c r="F5" s="14">
+        <v>209.51</v>
+      </c>
+      <c r="G5" t="s">
+        <v>212</v>
+      </c>
+      <c r="H5" t="s">
+        <v>215</v>
+      </c>
+      <c r="I5" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s">
         <v>218</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D6" t="s">
         <v>218</v>
       </c>
-      <c r="E5" s="20">
-        <f>F4</f>
+      <c r="E6" s="20">
+        <f>F5</f>
         <v>209.51</v>
       </c>
-      <c r="F5" s="20">
+      <c r="F6" s="20">
         <v>201.36</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G6" t="s">
         <v>219</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H6" t="s">
         <v>217</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I6" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B7" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="25" t="s">
+      <c r="C7" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D7" t="s">
         <v>196</v>
       </c>
-      <c r="E6" s="17">
+      <c r="E7" s="17">
         <v>201.36</v>
       </c>
-      <c r="F6" s="13">
+      <c r="F7" s="13">
         <v>196.18</v>
       </c>
-      <c r="G6" s="28" t="s">
+      <c r="G7" s="28" t="s">
         <v>200</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H7" t="s">
         <v>194</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I7" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
+    <row r="8" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
         <v>176</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" t="s">
-        <v>84</v>
-      </c>
-      <c r="D7" t="s">
-        <v>84</v>
-      </c>
-      <c r="E7" s="14">
-        <v>214.03</v>
-      </c>
-      <c r="F7" s="14">
-        <v>209.51</v>
-      </c>
-      <c r="G7" s="16" t="s">
-        <v>180</v>
-      </c>
-      <c r="H7" s="16" t="s">
-        <v>182</v>
-      </c>
-      <c r="I7" s="16" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="6" t="s">
-        <v>179</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>28</v>
       </c>
       <c r="C8" t="s">
+        <v>84</v>
+      </c>
+      <c r="D8" t="s">
+        <v>84</v>
+      </c>
+      <c r="E8" s="14">
+        <v>214.03</v>
+      </c>
+      <c r="F8" s="14">
+        <v>209.51</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="H8" s="16" t="s">
+        <v>182</v>
+      </c>
+      <c r="I8" s="16" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" t="s">
         <v>203</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D9" t="s">
         <v>203</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E9" s="13">
         <v>149.24</v>
       </c>
-      <c r="F8" s="13">
+      <c r="F9" s="13">
         <v>146.16999999999999</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G9" t="s">
         <v>204</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H9" t="s">
         <v>205</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I9" t="s">
         <v>209</v>
       </c>
     </row>
@@ -3100,7 +3148,7 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3244,25 +3292,28 @@
       <c r="C5" s="15">
         <v>159.27000000000001</v>
       </c>
-      <c r="D5" s="14">
-        <v>154.78</v>
+      <c r="D5" s="15">
+        <v>157.01</v>
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
-        <v>157.02500000000001</v>
+        <v>158.13999999999999</v>
       </c>
       <c r="F5">
         <f t="shared" si="1"/>
-        <v>10.855000000000018</v>
+        <v>11.969999999999999</v>
       </c>
       <c r="G5">
         <f t="shared" si="2"/>
-        <v>8.6100000000000136</v>
+        <v>10.840000000000003</v>
       </c>
       <c r="H5">
         <f t="shared" si="3"/>
         <v>13.100000000000023</v>
       </c>
+      <c r="I5" t="s">
+        <v>255</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
@@ -3293,6 +3344,9 @@
         <f t="shared" si="3"/>
         <v>67.860000000000014</v>
       </c>
+      <c r="I6" t="s">
+        <v>255</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
@@ -3301,19 +3355,19 @@
       <c r="B7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="15">
-        <v>217.49</v>
+      <c r="C7" s="14">
+        <v>214.03</v>
       </c>
       <c r="D7" s="14">
         <v>209.51</v>
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>213.5</v>
+        <v>211.76999999999998</v>
       </c>
       <c r="F7">
         <f t="shared" si="1"/>
-        <v>67.330000000000013</v>
+        <v>65.599999999999994</v>
       </c>
       <c r="G7">
         <f t="shared" si="2"/>
@@ -3321,7 +3375,10 @@
       </c>
       <c r="H7">
         <f t="shared" si="3"/>
-        <v>71.320000000000022</v>
+        <v>67.860000000000014</v>
+      </c>
+      <c r="I7" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -3594,7 +3651,7 @@
         <v>89.830000000000013</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>31</v>
       </c>
@@ -3624,7 +3681,7 @@
         <v>67.860000000000014</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>39</v>
       </c>
@@ -3654,7 +3711,7 @@
         <v>71.320000000000022</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>36</v>
       </c>
@@ -3684,7 +3741,7 @@
         <v>71.320000000000022</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
         <v>44</v>
       </c>
@@ -3714,7 +3771,7 @@
         <v>85.230000000000018</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="10" t="s">
         <v>33</v>
       </c>
@@ -3744,7 +3801,7 @@
         <v>67.860000000000014</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="7" t="s">
         <v>52</v>
       </c>
@@ -3775,7 +3832,7 @@
         <v>59.27000000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="8" t="s">
         <v>45</v>
       </c>
@@ -3805,7 +3862,7 @@
         <v>87.43</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="10" t="s">
         <v>40</v>
       </c>
@@ -3834,8 +3891,11 @@
         <f t="shared" si="3"/>
         <v>71.320000000000022</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I24" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="18" t="s">
         <v>90</v>
       </c>
@@ -3865,7 +3925,7 @@
         <v>87.43</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="9" t="s">
         <v>32</v>
       </c>
@@ -3905,10 +3965,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4280E281-9E32-4F6D-A0EF-078B3D4FF18C}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3977,55 +4037,55 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="14">
+        <v>214.03</v>
+      </c>
+      <c r="D3" s="14">
+        <v>209.51</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E5" si="0">(C3+D3)/2</f>
+        <v>211.76999999999998</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F5" si="1">E3-146.17</f>
+        <v>65.599999999999994</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G4" si="2">D3-146.17</f>
+        <v>63.34</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H4" si="3">C3-146.17</f>
+        <v>67.860000000000014</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="20">
+      <c r="C4" s="20">
         <v>227.3</v>
       </c>
-      <c r="D3" s="20">
-        <v>209.51</v>
-      </c>
-      <c r="E3">
-        <f t="shared" ref="E3:E8" si="0">(C3+D3)/2</f>
-        <v>218.405</v>
-      </c>
-      <c r="F3">
-        <f t="shared" ref="F3:F8" si="1">E3-146.17</f>
-        <v>72.235000000000014</v>
-      </c>
-      <c r="G3">
-        <f t="shared" ref="G3:G8" si="2">D3-146.17</f>
-        <v>63.34</v>
-      </c>
-      <c r="H3">
-        <f t="shared" ref="H3:H8" si="3">C3-146.17</f>
-        <v>81.130000000000024</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4" s="15">
-        <v>217.49</v>
-      </c>
-      <c r="D4" s="14">
+      <c r="D4" s="20">
         <v>209.51</v>
       </c>
       <c r="E4">
         <f t="shared" si="0"/>
-        <v>213.5</v>
+        <v>218.405</v>
       </c>
       <c r="F4">
         <f t="shared" si="1"/>
-        <v>67.330000000000013</v>
+        <v>72.235000000000014</v>
       </c>
       <c r="G4">
         <f t="shared" si="2"/>
@@ -4033,126 +4093,156 @@
       </c>
       <c r="H4">
         <f t="shared" si="3"/>
-        <v>71.320000000000022</v>
+        <v>81.130000000000024</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="20">
+      <c r="C5" s="15">
+        <v>217.49</v>
+      </c>
+      <c r="D5" s="14">
         <v>209.51</v>
-      </c>
-      <c r="D5" s="20">
-        <v>201.36</v>
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
-        <v>205.435</v>
+        <v>213.5</v>
       </c>
       <c r="F5">
         <f t="shared" si="1"/>
+        <v>67.330000000000013</v>
+      </c>
+      <c r="G5">
+        <f t="shared" ref="G3:G5" si="4">D5-146.17</f>
+        <v>63.34</v>
+      </c>
+      <c r="H5">
+        <f t="shared" ref="H4:H9" si="5">C5-146.17</f>
+        <v>71.320000000000022</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="20">
+        <v>209.51</v>
+      </c>
+      <c r="D6" s="20">
+        <v>201.36</v>
+      </c>
+      <c r="E6">
+        <f t="shared" ref="E4:E9" si="6">(C6+D6)/2</f>
+        <v>205.435</v>
+      </c>
+      <c r="F6">
+        <f t="shared" ref="F4:F9" si="7">E6-146.17</f>
         <v>59.265000000000015</v>
       </c>
-      <c r="G5">
-        <f t="shared" si="2"/>
+      <c r="G6">
+        <f t="shared" ref="G4:G9" si="8">D6-146.17</f>
         <v>55.190000000000026</v>
       </c>
-      <c r="H5">
-        <f t="shared" si="3"/>
+      <c r="H6">
+        <f t="shared" si="5"/>
         <v>63.34</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
         <v>249</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B7" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="17">
+      <c r="C7" s="17">
         <v>201.36</v>
       </c>
-      <c r="D6" s="13">
+      <c r="D7" s="13">
         <v>196.18</v>
       </c>
-      <c r="E6">
-        <f t="shared" si="0"/>
+      <c r="E7">
+        <f t="shared" si="6"/>
         <v>198.77</v>
       </c>
-      <c r="F6">
-        <f t="shared" si="1"/>
+      <c r="F7">
+        <f t="shared" si="7"/>
         <v>52.600000000000023</v>
       </c>
-      <c r="G6">
-        <f t="shared" si="2"/>
+      <c r="G7">
+        <f t="shared" si="8"/>
         <v>50.010000000000019</v>
       </c>
-      <c r="H6">
-        <f t="shared" si="3"/>
+      <c r="H7">
+        <f t="shared" si="5"/>
         <v>55.190000000000026</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
+    <row r="8" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
         <v>250</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" s="14">
-        <v>214.03</v>
-      </c>
-      <c r="D7" s="14">
-        <v>209.51</v>
-      </c>
-      <c r="E7">
-        <f t="shared" si="0"/>
-        <v>211.76999999999998</v>
-      </c>
-      <c r="F7">
-        <f t="shared" si="1"/>
-        <v>65.599999999999994</v>
-      </c>
-      <c r="G7">
-        <f t="shared" si="2"/>
-        <v>63.34</v>
-      </c>
-      <c r="H7">
-        <f t="shared" si="3"/>
-        <v>67.860000000000014</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="6" t="s">
-        <v>251</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="13">
+      <c r="C8" s="14">
+        <v>214.03</v>
+      </c>
+      <c r="D8" s="14">
+        <v>209.51</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="6"/>
+        <v>211.76999999999998</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="7"/>
+        <v>65.599999999999994</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="8"/>
+        <v>63.34</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="5"/>
+        <v>67.860000000000014</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="13">
         <v>149.24</v>
       </c>
-      <c r="D8" s="13">
+      <c r="D9" s="13">
         <v>146.16999999999999</v>
       </c>
-      <c r="E8">
-        <f t="shared" si="0"/>
+      <c r="E9">
+        <f t="shared" si="6"/>
         <v>147.70499999999998</v>
       </c>
-      <c r="F8">
-        <f t="shared" si="1"/>
+      <c r="F9">
+        <f t="shared" si="7"/>
         <v>1.5349999999999966</v>
       </c>
-      <c r="G8">
-        <f t="shared" si="2"/>
+      <c r="G9">
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="H8">
-        <f t="shared" si="3"/>
+      <c r="H9">
+        <f t="shared" si="5"/>
         <v>3.0700000000000216</v>
       </c>
     </row>

</xml_diff>